<commit_message>
updated HPLC standards analysis
</commit_message>
<xml_diff>
--- a/Metabolites/HPLC/Data/information_HPLC.xlsx
+++ b/Metabolites/HPLC/Data/information_HPLC.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Plan de Plaque" sheetId="1" state="visible" r:id="rId3"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="482" uniqueCount="239">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="564" uniqueCount="236">
   <si>
     <t xml:space="preserve">Cette feuille décrit les informations du plan de plaque. Elle n'est pas utilisée pour les analyses, mais est utile à l'expérimentateur pour décrire l'organisation des échantillons dans la plaque.</t>
   </si>
@@ -150,13 +150,16 @@
     <t xml:space="preserve">STD12-GS2-0.06</t>
   </si>
   <si>
+    <t xml:space="preserve">Cette fiche définit les noms des solutions étalons et la concentration de chaque composé dans les standards. Les mêmes noms d'échantillons doivent être utilisés pour les standards de la fiche « Samples ».</t>
+  </si>
+  <si>
     <t xml:space="preserve">Sample</t>
   </si>
   <si>
     <t xml:space="preserve">Compound</t>
   </si>
   <si>
-    <t xml:space="preserve">mM</t>
+    <t xml:space="preserve">Concentration_mM</t>
   </si>
   <si>
     <t xml:space="preserve">STD1_100</t>
@@ -213,19 +216,37 @@
     <t xml:space="preserve">STD2_06</t>
   </si>
   <si>
-    <t xml:space="preserve">STD12_100</t>
-  </si>
-  <si>
-    <t xml:space="preserve">STD12_50</t>
-  </si>
-  <si>
-    <t xml:space="preserve">STD12_25</t>
-  </si>
-  <si>
-    <t xml:space="preserve">STD12_12</t>
-  </si>
-  <si>
-    <t xml:space="preserve">STD12_06</t>
+    <t xml:space="preserve">STD12_100_water</t>
+  </si>
+  <si>
+    <t xml:space="preserve">STD12_50_water</t>
+  </si>
+  <si>
+    <t xml:space="preserve">STD12_25_water</t>
+  </si>
+  <si>
+    <t xml:space="preserve">STD12_12_water</t>
+  </si>
+  <si>
+    <t xml:space="preserve">STD12_06_water</t>
+  </si>
+  <si>
+    <t xml:space="preserve">STD12_100_GS2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">STD12_50_GS2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">STD12_25_GS2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">STD12_12_GS2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">STD12_06_GS2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cette feuille fait la correspondance entre les noms de fichiers et les descriptions des échantillons. Les descriptions des standards doivent être les mêmes que sur la feuille "Standards".</t>
   </si>
   <si>
     <t xml:space="preserve">File</t>
@@ -486,9 +507,6 @@
     <t xml:space="preserve">C:\LabSolutions\Data\Loïc\2024-11-19\F4.lcd</t>
   </si>
   <si>
-    <t xml:space="preserve">STD12_100_water</t>
-  </si>
-  <si>
     <t xml:space="preserve">B2.2.lcd</t>
   </si>
   <si>
@@ -516,9 +534,6 @@
     <t xml:space="preserve">C:\LabSolutions\Data\Loïc\2024-11-19\blanc7.lcd</t>
   </si>
   <si>
-    <t xml:space="preserve">STD12_50_water</t>
-  </si>
-  <si>
     <t xml:space="preserve">B5.2.lcd</t>
   </si>
   <si>
@@ -537,9 +552,6 @@
     <t xml:space="preserve">C:\LabSolutions\Data\Loïc\2024-11-19\B7.2.lcd</t>
   </si>
   <si>
-    <t xml:space="preserve">STD12_25_water</t>
-  </si>
-  <si>
     <t xml:space="preserve">B8.2.lcd</t>
   </si>
   <si>
@@ -567,9 +579,6 @@
     <t xml:space="preserve">C:\LabSolutions\Data\Loïc\2024-11-19\blanc8.lcd</t>
   </si>
   <si>
-    <t xml:space="preserve">STD12_12_water</t>
-  </si>
-  <si>
     <t xml:space="preserve">C2.2.lcd</t>
   </si>
   <si>
@@ -588,9 +597,6 @@
     <t xml:space="preserve">C:\LabSolutions\Data\Loïc\2024-11-19\C4.2.lcd</t>
   </si>
   <si>
-    <t xml:space="preserve">STD12_06_water</t>
-  </si>
-  <si>
     <t xml:space="preserve">C5.2.lcd</t>
   </si>
   <si>
@@ -618,9 +624,6 @@
     <t xml:space="preserve">C:\LabSolutions\Data\Loïc\2024-11-19\blanc9.lcd</t>
   </si>
   <si>
-    <t xml:space="preserve">STD12_100_GS2</t>
-  </si>
-  <si>
     <t xml:space="preserve">D2.2.lcd</t>
   </si>
   <si>
@@ -639,9 +642,6 @@
     <t xml:space="preserve">C:\LabSolutions\Data\Loïc\2024-11-19\D4.2.lcd</t>
   </si>
   <si>
-    <t xml:space="preserve">STD12_50_GS2</t>
-  </si>
-  <si>
     <t xml:space="preserve">D5.2.lcd</t>
   </si>
   <si>
@@ -669,9 +669,6 @@
     <t xml:space="preserve">C:\LabSolutions\Data\Loïc\2024-11-19\blanc10.lcd</t>
   </si>
   <si>
-    <t xml:space="preserve">STD12_25_GS2</t>
-  </si>
-  <si>
     <t xml:space="preserve">D8.2.lcd</t>
   </si>
   <si>
@@ -690,9 +687,6 @@
     <t xml:space="preserve">C:\LabSolutions\Data\Loïc\2024-11-19\D10.2.lcd</t>
   </si>
   <si>
-    <t xml:space="preserve">STD12_12_GS2</t>
-  </si>
-  <si>
     <t xml:space="preserve">E2.2.lcd</t>
   </si>
   <si>
@@ -718,9 +712,6 @@
   </si>
   <si>
     <t xml:space="preserve">C:\LabSolutions\Data\Loïc\2024-11-19\blanc11.lcd</t>
-  </si>
-  <si>
-    <t xml:space="preserve">STD12_06_GS2</t>
   </si>
   <si>
     <t xml:space="preserve">E5.2.lcd</t>
@@ -748,7 +739,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="12">
+  <fonts count="11">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -805,14 +796,6 @@
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="0"/>
       <charset val="1"/>
     </font>
     <font>
@@ -894,7 +877,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="17">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -939,39 +922,27 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -3291,1099 +3262,1388 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D1000"/>
+  <dimension ref="A1:G1002"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G9" activeCellId="0" sqref="G9"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A97" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I90" activeCellId="0" sqref="I90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.4296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="11" width="18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="18"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="14.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="23.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="4" style="1" width="14.43"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="12" t="s">
+    <row r="1" customFormat="false" ht="26.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="B1" s="12" t="s">
-        <v>43</v>
-      </c>
-      <c r="C1" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="D1" s="12"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="13" t="s">
-        <v>45</v>
-      </c>
-      <c r="B2" s="13" t="s">
-        <v>46</v>
-      </c>
-      <c r="C2" s="14" t="n">
-        <v>50</v>
-      </c>
-      <c r="D2" s="13"/>
+      <c r="A2" s="12"/>
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="C3" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="B3" s="13" t="s">
+      <c r="D3" s="12"/>
+    </row>
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>47</v>
-      </c>
-      <c r="C3" s="14" t="n">
-        <v>50</v>
-      </c>
-      <c r="D3" s="13"/>
-    </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="13" t="s">
-        <v>45</v>
-      </c>
-      <c r="B4" s="13" t="s">
-        <v>48</v>
       </c>
       <c r="C4" s="14" t="n">
         <v>50</v>
       </c>
-      <c r="D4" s="13"/>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="13" t="s">
-        <v>45</v>
-      </c>
-      <c r="B5" s="13" t="s">
+      <c r="A5" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C5" s="14" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C5" s="14" t="n">
+      <c r="C6" s="14" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C7" s="14" t="n">
         <v>342.5</v>
       </c>
-      <c r="D5" s="13"/>
-    </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="13" t="s">
-        <v>45</v>
-      </c>
-      <c r="B6" s="13" t="s">
-        <v>50</v>
-      </c>
-      <c r="C6" s="14" t="n">
+    </row>
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C8" s="14" t="n">
         <v>27.775</v>
       </c>
-      <c r="D6" s="13"/>
-    </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="13" t="s">
-        <v>51</v>
-      </c>
-      <c r="B7" s="13" t="s">
-        <v>46</v>
-      </c>
-      <c r="C7" s="14" t="n">
-        <f aca="false">C2/2</f>
-        <v>25</v>
-      </c>
-      <c r="D7" s="13"/>
-    </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="13" t="s">
-        <v>51</v>
-      </c>
-      <c r="B8" s="13" t="s">
+    </row>
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>47</v>
-      </c>
-      <c r="C8" s="14" t="n">
-        <f aca="false">C3/2</f>
-        <v>25</v>
-      </c>
-      <c r="D8" s="13"/>
-    </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="13" t="s">
-        <v>51</v>
-      </c>
-      <c r="B9" s="13" t="s">
-        <v>48</v>
       </c>
       <c r="C9" s="14" t="n">
         <f aca="false">C4/2</f>
         <v>25</v>
       </c>
-      <c r="D9" s="13"/>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="13" t="s">
-        <v>51</v>
-      </c>
-      <c r="B10" s="13" t="s">
-        <v>49</v>
+      <c r="A10" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>48</v>
       </c>
       <c r="C10" s="14" t="n">
         <f aca="false">C5/2</f>
-        <v>171.25</v>
-      </c>
-      <c r="D10" s="13"/>
+        <v>25</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="13" t="s">
-        <v>51</v>
-      </c>
-      <c r="B11" s="13" t="s">
-        <v>50</v>
+      <c r="A11" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>49</v>
       </c>
       <c r="C11" s="14" t="n">
         <f aca="false">C6/2</f>
-        <v>13.8875</v>
-      </c>
-      <c r="D11" s="13"/>
+        <v>25</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="13" t="s">
+      <c r="A12" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B12" s="13" t="s">
-        <v>46</v>
+      <c r="B12" s="1" t="s">
+        <v>50</v>
       </c>
       <c r="C12" s="14" t="n">
         <f aca="false">C7/2</f>
-        <v>12.5</v>
-      </c>
-      <c r="D12" s="13"/>
+        <v>171.25</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="13" t="s">
+      <c r="A13" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B13" s="13" t="s">
-        <v>47</v>
+      <c r="B13" s="1" t="s">
+        <v>51</v>
       </c>
       <c r="C13" s="14" t="n">
         <f aca="false">C8/2</f>
-        <v>12.5</v>
-      </c>
-      <c r="D13" s="13"/>
+        <v>13.8875</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="13" t="s">
-        <v>52</v>
-      </c>
-      <c r="B14" s="13" t="s">
-        <v>48</v>
+      <c r="A14" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>47</v>
       </c>
       <c r="C14" s="14" t="n">
         <f aca="false">C9/2</f>
         <v>12.5</v>
       </c>
-      <c r="D14" s="13"/>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="13" t="s">
-        <v>52</v>
-      </c>
-      <c r="B15" s="13" t="s">
-        <v>49</v>
+      <c r="A15" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>48</v>
       </c>
       <c r="C15" s="14" t="n">
         <f aca="false">C10/2</f>
-        <v>85.625</v>
-      </c>
-      <c r="D15" s="13"/>
+        <v>12.5</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="13" t="s">
-        <v>52</v>
-      </c>
-      <c r="B16" s="13" t="s">
-        <v>50</v>
+      <c r="A16" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>49</v>
       </c>
       <c r="C16" s="14" t="n">
         <f aca="false">C11/2</f>
-        <v>6.94375</v>
-      </c>
-      <c r="D16" s="13"/>
+        <v>12.5</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="13" t="s">
+      <c r="A17" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B17" s="13" t="s">
-        <v>46</v>
+      <c r="B17" s="1" t="s">
+        <v>50</v>
       </c>
       <c r="C17" s="14" t="n">
         <f aca="false">C12/2</f>
-        <v>6.25</v>
-      </c>
-      <c r="D17" s="13"/>
+        <v>85.625</v>
+      </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="13" t="s">
+      <c r="A18" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B18" s="13" t="s">
-        <v>47</v>
+      <c r="B18" s="1" t="s">
+        <v>51</v>
       </c>
       <c r="C18" s="14" t="n">
         <f aca="false">C13/2</f>
-        <v>6.25</v>
-      </c>
-      <c r="D18" s="13"/>
+        <v>6.94375</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="13" t="s">
-        <v>53</v>
-      </c>
-      <c r="B19" s="13" t="s">
-        <v>48</v>
+      <c r="A19" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>47</v>
       </c>
       <c r="C19" s="14" t="n">
         <f aca="false">C14/2</f>
         <v>6.25</v>
       </c>
-      <c r="D19" s="13"/>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="13" t="s">
-        <v>53</v>
-      </c>
-      <c r="B20" s="13" t="s">
-        <v>49</v>
+      <c r="A20" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>48</v>
       </c>
       <c r="C20" s="14" t="n">
         <f aca="false">C15/2</f>
-        <v>42.8125</v>
-      </c>
-      <c r="D20" s="13"/>
+        <v>6.25</v>
+      </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="13" t="s">
-        <v>53</v>
-      </c>
-      <c r="B21" s="13" t="s">
-        <v>50</v>
+      <c r="A21" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>49</v>
       </c>
       <c r="C21" s="14" t="n">
         <f aca="false">C16/2</f>
-        <v>3.471875</v>
-      </c>
-      <c r="D21" s="13"/>
+        <v>6.25</v>
+      </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="13" t="s">
+      <c r="A22" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B22" s="13" t="s">
-        <v>46</v>
+      <c r="B22" s="1" t="s">
+        <v>50</v>
       </c>
       <c r="C22" s="14" t="n">
         <f aca="false">C17/2</f>
-        <v>3.125</v>
-      </c>
-      <c r="D22" s="13"/>
+        <v>42.8125</v>
+      </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="13" t="s">
+      <c r="A23" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B23" s="13" t="s">
-        <v>47</v>
+      <c r="B23" s="1" t="s">
+        <v>51</v>
       </c>
       <c r="C23" s="14" t="n">
         <f aca="false">C18/2</f>
-        <v>3.125</v>
-      </c>
-      <c r="D23" s="13"/>
+        <v>3.471875</v>
+      </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="13" t="s">
-        <v>54</v>
-      </c>
-      <c r="B24" s="13" t="s">
-        <v>48</v>
+      <c r="A24" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>47</v>
       </c>
       <c r="C24" s="14" t="n">
         <f aca="false">C19/2</f>
         <v>3.125</v>
       </c>
-      <c r="D24" s="13"/>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="13" t="s">
-        <v>54</v>
-      </c>
-      <c r="B25" s="13" t="s">
-        <v>49</v>
+      <c r="A25" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>48</v>
       </c>
       <c r="C25" s="14" t="n">
         <f aca="false">C20/2</f>
-        <v>21.40625</v>
-      </c>
-      <c r="D25" s="13"/>
+        <v>3.125</v>
+      </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="13" t="s">
-        <v>54</v>
-      </c>
-      <c r="B26" s="13" t="s">
-        <v>50</v>
+      <c r="A26" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>49</v>
       </c>
       <c r="C26" s="14" t="n">
         <f aca="false">C21/2</f>
+        <v>3.125</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C27" s="14" t="n">
+        <f aca="false">C22/2</f>
+        <v>21.40625</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C28" s="14" t="n">
+        <f aca="false">C23/2</f>
         <v>1.7359375</v>
       </c>
-      <c r="D26" s="13"/>
-    </row>
-    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="13" t="s">
-        <v>55</v>
-      </c>
-      <c r="B27" s="13" t="s">
+    </row>
+    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="C27" s="14" t="n">
-        <v>50</v>
-      </c>
-      <c r="D27" s="13"/>
-    </row>
-    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="13" t="s">
-        <v>55</v>
-      </c>
-      <c r="B28" s="13" t="s">
+      <c r="B29" s="1" t="s">
         <v>57</v>
-      </c>
-      <c r="C28" s="14" t="n">
-        <v>50</v>
-      </c>
-      <c r="D28" s="13"/>
-    </row>
-    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="13" t="s">
-        <v>55</v>
-      </c>
-      <c r="B29" s="13" t="s">
-        <v>58</v>
       </c>
       <c r="C29" s="14" t="n">
         <v>50</v>
       </c>
-      <c r="D29" s="13"/>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="13" t="s">
+      <c r="A30" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C30" s="14" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B31" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="B30" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="C30" s="14" t="n">
+      <c r="C31" s="14" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C32" s="14" t="n">
         <v>25</v>
       </c>
-      <c r="D30" s="13"/>
-    </row>
-    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="13" t="s">
+    </row>
+    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C33" s="14" t="n">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B34" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="B31" s="13" t="s">
+      <c r="C34" s="1" t="n">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B35" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="C31" s="14" t="n">
-        <v>25</v>
-      </c>
-      <c r="D31" s="13"/>
-    </row>
-    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="13" t="s">
+      <c r="C35" s="1" t="n">
+        <v>12.5</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C36" s="1" t="n">
+        <v>12.5</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B37" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="B32" s="13" t="s">
+      <c r="C37" s="1" t="n">
+        <v>12.5</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C38" s="1" t="n">
+        <v>6.25</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B39" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="C32" s="13" t="n">
-        <v>25</v>
-      </c>
-      <c r="D32" s="13"/>
-    </row>
-    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="13" t="s">
-        <v>60</v>
-      </c>
-      <c r="B33" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="C33" s="13" t="n">
-        <v>12.5</v>
-      </c>
-      <c r="D33" s="13"/>
-    </row>
-    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="13" t="s">
-        <v>60</v>
-      </c>
-      <c r="B34" s="13" t="s">
+      <c r="C39" s="1" t="n">
+        <v>6.25</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C40" s="1" t="n">
+        <v>6.25</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B41" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="C34" s="13" t="n">
-        <v>12.5</v>
-      </c>
-      <c r="D34" s="13"/>
-    </row>
-    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="13" t="s">
-        <v>60</v>
-      </c>
-      <c r="B35" s="13" t="s">
+      <c r="C41" s="1" t="n">
+        <v>3.125</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B42" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="C35" s="13" t="n">
-        <v>12.5</v>
-      </c>
-      <c r="D35" s="13"/>
-    </row>
-    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="13" t="s">
-        <v>61</v>
-      </c>
-      <c r="B36" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="C36" s="13" t="n">
-        <v>6.25</v>
-      </c>
-      <c r="D36" s="13"/>
-    </row>
-    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="13" t="s">
-        <v>61</v>
-      </c>
-      <c r="B37" s="13" t="s">
+      <c r="C42" s="1" t="n">
+        <v>3.125</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C43" s="1" t="n">
+        <v>3.125</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C44" s="1" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C45" s="1" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C46" s="1" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C47" s="1" t="n">
+        <v>342.5</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C48" s="14" t="n">
+        <v>27.775</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B49" s="1" t="s">
         <v>57</v>
-      </c>
-      <c r="C37" s="13" t="n">
-        <v>6.25</v>
-      </c>
-      <c r="D37" s="13"/>
-    </row>
-    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="13" t="s">
-        <v>61</v>
-      </c>
-      <c r="B38" s="13" t="s">
-        <v>58</v>
-      </c>
-      <c r="C38" s="13" t="n">
-        <v>6.25</v>
-      </c>
-      <c r="D38" s="13"/>
-    </row>
-    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="13" t="s">
-        <v>62</v>
-      </c>
-      <c r="B39" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="C39" s="13" t="n">
-        <v>3.125</v>
-      </c>
-      <c r="D39" s="13"/>
-    </row>
-    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="13" t="s">
-        <v>62</v>
-      </c>
-      <c r="B40" s="13" t="s">
-        <v>57</v>
-      </c>
-      <c r="C40" s="13" t="n">
-        <v>3.125</v>
-      </c>
-      <c r="D40" s="13"/>
-    </row>
-    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="13" t="s">
-        <v>62</v>
-      </c>
-      <c r="B41" s="13" t="s">
-        <v>58</v>
-      </c>
-      <c r="C41" s="13" t="n">
-        <v>3.125</v>
-      </c>
-      <c r="D41" s="13"/>
-    </row>
-    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="B42" s="13" t="s">
-        <v>46</v>
-      </c>
-      <c r="C42" s="13" t="n">
-        <v>50</v>
-      </c>
-      <c r="D42" s="13"/>
-    </row>
-    <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="B43" s="13" t="s">
-        <v>47</v>
-      </c>
-      <c r="C43" s="13" t="n">
-        <v>50</v>
-      </c>
-      <c r="D43" s="13"/>
-    </row>
-    <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="B44" s="13" t="s">
-        <v>48</v>
-      </c>
-      <c r="C44" s="13" t="n">
-        <v>50</v>
-      </c>
-      <c r="D44" s="13"/>
-    </row>
-    <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="B45" s="13" t="s">
-        <v>49</v>
-      </c>
-      <c r="C45" s="13" t="n">
-        <v>342.5</v>
-      </c>
-      <c r="D45" s="13"/>
-    </row>
-    <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="B46" s="13" t="s">
-        <v>50</v>
-      </c>
-      <c r="C46" s="14" t="n">
-        <v>27.775</v>
-      </c>
-      <c r="D46" s="13"/>
-    </row>
-    <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="B47" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="C47" s="14" t="n">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="B48" s="13" t="s">
-        <v>57</v>
-      </c>
-      <c r="C48" s="14" t="n">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="B49" s="13" t="s">
-        <v>58</v>
       </c>
       <c r="C49" s="14" t="n">
         <v>50</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="11" t="s">
+      <c r="A50" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="B50" s="13" t="s">
-        <v>46</v>
+      <c r="B50" s="1" t="s">
+        <v>58</v>
       </c>
       <c r="C50" s="14" t="n">
-        <v>25</v>
+        <v>50</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="11" t="s">
+      <c r="A51" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="B51" s="13" t="s">
+      <c r="B51" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C51" s="14" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B52" s="1" t="s">
         <v>47</v>
-      </c>
-      <c r="C51" s="14" t="n">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="B52" s="13" t="s">
-        <v>48</v>
       </c>
       <c r="C52" s="14" t="n">
         <v>25</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="B53" s="13" t="s">
+      <c r="A53" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C53" s="14" t="n">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B54" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C53" s="14" t="n">
+      <c r="C54" s="14" t="n">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C55" s="14" t="n">
         <v>171.25</v>
       </c>
     </row>
-    <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="B54" s="13" t="s">
-        <v>50</v>
-      </c>
-      <c r="C54" s="14" t="n">
+    <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C56" s="14" t="n">
         <v>13.8875</v>
       </c>
     </row>
-    <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="B55" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="C55" s="14" t="n">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="B56" s="13" t="s">
+    <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B57" s="1" t="s">
         <v>57</v>
-      </c>
-      <c r="C56" s="14" t="n">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="B57" s="13" t="s">
-        <v>58</v>
       </c>
       <c r="C57" s="14" t="n">
         <v>25</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="11" t="s">
+      <c r="A58" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="B58" s="13" t="s">
-        <v>46</v>
+      <c r="B58" s="1" t="s">
+        <v>58</v>
       </c>
       <c r="C58" s="14" t="n">
-        <v>12.5</v>
+        <v>25</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="11" t="s">
+      <c r="A59" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="B59" s="13" t="s">
+      <c r="B59" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C59" s="14" t="n">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B60" s="1" t="s">
         <v>47</v>
-      </c>
-      <c r="C59" s="14" t="n">
-        <v>12.5</v>
-      </c>
-    </row>
-    <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="11" t="s">
-        <v>65</v>
-      </c>
-      <c r="B60" s="13" t="s">
-        <v>48</v>
       </c>
       <c r="C60" s="14" t="n">
         <v>12.5</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="11" t="s">
-        <v>65</v>
-      </c>
-      <c r="B61" s="13" t="s">
+      <c r="A61" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C61" s="14" t="n">
+        <v>12.5</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B62" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C61" s="14" t="n">
+      <c r="C62" s="14" t="n">
+        <v>12.5</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C63" s="14" t="n">
         <v>85.625</v>
       </c>
     </row>
-    <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="11" t="s">
-        <v>65</v>
-      </c>
-      <c r="B62" s="13" t="s">
-        <v>50</v>
-      </c>
-      <c r="C62" s="14" t="n">
+    <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A64" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C64" s="14" t="n">
         <v>6.94375</v>
       </c>
     </row>
-    <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="11" t="s">
-        <v>65</v>
-      </c>
-      <c r="B63" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="C63" s="14" t="n">
-        <v>12.5</v>
-      </c>
-    </row>
-    <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="11" t="s">
-        <v>65</v>
-      </c>
-      <c r="B64" s="13" t="s">
+    <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A65" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B65" s="1" t="s">
         <v>57</v>
-      </c>
-      <c r="C64" s="14" t="n">
-        <v>12.5</v>
-      </c>
-    </row>
-    <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="11" t="s">
-        <v>65</v>
-      </c>
-      <c r="B65" s="13" t="s">
-        <v>58</v>
       </c>
       <c r="C65" s="14" t="n">
         <v>12.5</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="11" t="s">
+      <c r="A66" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B66" s="13" t="s">
-        <v>46</v>
+      <c r="B66" s="1" t="s">
+        <v>58</v>
       </c>
       <c r="C66" s="14" t="n">
-        <v>6.25</v>
+        <v>12.5</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="11" t="s">
+      <c r="A67" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B67" s="13" t="s">
+      <c r="B67" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C67" s="14" t="n">
+        <v>12.5</v>
+      </c>
+    </row>
+    <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A68" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B68" s="1" t="s">
         <v>47</v>
-      </c>
-      <c r="C67" s="14" t="n">
-        <v>6.25</v>
-      </c>
-    </row>
-    <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="11" t="s">
-        <v>66</v>
-      </c>
-      <c r="B68" s="13" t="s">
-        <v>48</v>
       </c>
       <c r="C68" s="14" t="n">
         <v>6.25</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="11" t="s">
-        <v>66</v>
-      </c>
-      <c r="B69" s="13" t="s">
+      <c r="A69" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C69" s="14" t="n">
+        <v>6.25</v>
+      </c>
+    </row>
+    <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A70" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B70" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C69" s="14" t="n">
+      <c r="C70" s="14" t="n">
+        <v>6.25</v>
+      </c>
+    </row>
+    <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A71" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C71" s="14" t="n">
         <v>42.8125</v>
       </c>
     </row>
-    <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A70" s="11" t="s">
-        <v>66</v>
-      </c>
-      <c r="B70" s="13" t="s">
-        <v>50</v>
-      </c>
-      <c r="C70" s="14" t="n">
+    <row r="72" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A72" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C72" s="14" t="n">
         <v>3.471875</v>
       </c>
     </row>
-    <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="11" t="s">
-        <v>66</v>
-      </c>
-      <c r="B71" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="C71" s="14" t="n">
-        <v>6.25</v>
-      </c>
-    </row>
-    <row r="72" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A72" s="11" t="s">
-        <v>66</v>
-      </c>
-      <c r="B72" s="13" t="s">
+    <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A73" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B73" s="1" t="s">
         <v>57</v>
-      </c>
-      <c r="C72" s="14" t="n">
-        <v>6.25</v>
-      </c>
-    </row>
-    <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A73" s="11" t="s">
-        <v>66</v>
-      </c>
-      <c r="B73" s="13" t="s">
-        <v>58</v>
       </c>
       <c r="C73" s="14" t="n">
         <v>6.25</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A74" s="11" t="s">
+      <c r="A74" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="B74" s="13" t="s">
-        <v>46</v>
+      <c r="B74" s="1" t="s">
+        <v>58</v>
       </c>
       <c r="C74" s="14" t="n">
-        <v>3.125</v>
+        <v>6.25</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A75" s="11" t="s">
+      <c r="A75" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="B75" s="13" t="s">
+      <c r="B75" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C75" s="14" t="n">
+        <v>6.25</v>
+      </c>
+    </row>
+    <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A76" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B76" s="1" t="s">
         <v>47</v>
-      </c>
-      <c r="C75" s="14" t="n">
-        <v>3.125</v>
-      </c>
-    </row>
-    <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A76" s="11" t="s">
-        <v>67</v>
-      </c>
-      <c r="B76" s="13" t="s">
-        <v>48</v>
       </c>
       <c r="C76" s="14" t="n">
         <v>3.125</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A77" s="11" t="s">
-        <v>67</v>
-      </c>
-      <c r="B77" s="13" t="s">
+      <c r="A77" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B77" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C77" s="14" t="n">
+        <v>3.125</v>
+      </c>
+    </row>
+    <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A78" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B78" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C77" s="14" t="n">
+      <c r="C78" s="14" t="n">
+        <v>3.125</v>
+      </c>
+    </row>
+    <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A79" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B79" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C79" s="14" t="n">
         <v>21.40625</v>
       </c>
     </row>
-    <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A78" s="11" t="s">
-        <v>67</v>
-      </c>
-      <c r="B78" s="13" t="s">
-        <v>50</v>
-      </c>
-      <c r="C78" s="14" t="n">
+    <row r="80" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A80" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B80" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C80" s="14" t="n">
         <v>1.7359375</v>
       </c>
     </row>
-    <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A79" s="11" t="s">
-        <v>67</v>
-      </c>
-      <c r="B79" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="C79" s="14" t="n">
-        <v>3.125</v>
-      </c>
-    </row>
-    <row r="80" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A80" s="11" t="s">
-        <v>67</v>
-      </c>
-      <c r="B80" s="13" t="s">
+    <row r="81" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A81" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B81" s="1" t="s">
         <v>57</v>
-      </c>
-      <c r="C80" s="14" t="n">
-        <v>3.125</v>
-      </c>
-    </row>
-    <row r="81" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A81" s="11" t="s">
-        <v>67</v>
-      </c>
-      <c r="B81" s="13" t="s">
-        <v>58</v>
       </c>
       <c r="C81" s="14" t="n">
         <v>3.125</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C82" s="14"/>
+      <c r="A82" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B82" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C82" s="14" t="n">
+        <v>3.125</v>
+      </c>
     </row>
     <row r="83" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C83" s="14"/>
+      <c r="A83" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B83" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C83" s="14" t="n">
+        <v>3.125</v>
+      </c>
     </row>
     <row r="84" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C84" s="14"/>
+      <c r="A84" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B84" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C84" s="1" t="n">
+        <v>50</v>
+      </c>
     </row>
     <row r="85" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C85" s="14"/>
+      <c r="A85" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B85" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C85" s="1" t="n">
+        <v>50</v>
+      </c>
     </row>
     <row r="86" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C86" s="14"/>
+      <c r="A86" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B86" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C86" s="1" t="n">
+        <v>50</v>
+      </c>
     </row>
     <row r="87" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C87" s="14"/>
+      <c r="A87" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B87" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C87" s="1" t="n">
+        <v>342.5</v>
+      </c>
     </row>
     <row r="88" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C88" s="14"/>
+      <c r="A88" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B88" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C88" s="14" t="n">
+        <v>27.775</v>
+      </c>
     </row>
     <row r="89" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C89" s="14"/>
+      <c r="A89" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B89" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C89" s="14" t="n">
+        <v>50</v>
+      </c>
     </row>
     <row r="90" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C90" s="14"/>
+      <c r="A90" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B90" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C90" s="14" t="n">
+        <v>50</v>
+      </c>
     </row>
     <row r="91" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C91" s="14"/>
+      <c r="A91" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B91" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C91" s="14" t="n">
+        <v>50</v>
+      </c>
     </row>
     <row r="92" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C92" s="14"/>
+      <c r="A92" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B92" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C92" s="14" t="n">
+        <v>25</v>
+      </c>
     </row>
     <row r="93" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C93" s="14"/>
+      <c r="A93" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B93" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C93" s="14" t="n">
+        <v>25</v>
+      </c>
     </row>
     <row r="94" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C94" s="14"/>
+      <c r="A94" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B94" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C94" s="14" t="n">
+        <v>25</v>
+      </c>
     </row>
     <row r="95" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C95" s="14"/>
+      <c r="A95" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B95" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C95" s="14" t="n">
+        <v>171.25</v>
+      </c>
     </row>
     <row r="96" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C96" s="14"/>
+      <c r="A96" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B96" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C96" s="14" t="n">
+        <v>13.8875</v>
+      </c>
     </row>
     <row r="97" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C97" s="14"/>
+      <c r="A97" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B97" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C97" s="14" t="n">
+        <v>25</v>
+      </c>
     </row>
     <row r="98" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C98" s="14"/>
+      <c r="A98" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B98" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C98" s="14" t="n">
+        <v>25</v>
+      </c>
     </row>
     <row r="99" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C99" s="14"/>
+      <c r="A99" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B99" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C99" s="14" t="n">
+        <v>25</v>
+      </c>
     </row>
     <row r="100" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C100" s="14"/>
+      <c r="A100" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B100" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C100" s="14" t="n">
+        <v>12.5</v>
+      </c>
     </row>
     <row r="101" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C101" s="14"/>
+      <c r="A101" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B101" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C101" s="14" t="n">
+        <v>12.5</v>
+      </c>
     </row>
     <row r="102" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C102" s="14"/>
+      <c r="A102" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B102" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C102" s="14" t="n">
+        <v>12.5</v>
+      </c>
     </row>
     <row r="103" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C103" s="14"/>
+      <c r="A103" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B103" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C103" s="14" t="n">
+        <v>85.625</v>
+      </c>
     </row>
     <row r="104" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C104" s="14"/>
+      <c r="A104" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B104" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C104" s="14" t="n">
+        <v>6.94375</v>
+      </c>
     </row>
     <row r="105" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C105" s="14"/>
+      <c r="A105" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B105" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C105" s="14" t="n">
+        <v>12.5</v>
+      </c>
     </row>
     <row r="106" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C106" s="14"/>
+      <c r="A106" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B106" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C106" s="14" t="n">
+        <v>12.5</v>
+      </c>
     </row>
     <row r="107" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C107" s="14"/>
+      <c r="A107" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B107" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C107" s="14" t="n">
+        <v>12.5</v>
+      </c>
     </row>
     <row r="108" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C108" s="14"/>
+      <c r="A108" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B108" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C108" s="14" t="n">
+        <v>6.25</v>
+      </c>
     </row>
     <row r="109" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C109" s="14"/>
+      <c r="A109" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B109" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C109" s="14" t="n">
+        <v>6.25</v>
+      </c>
     </row>
     <row r="110" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C110" s="14"/>
+      <c r="A110" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B110" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C110" s="14" t="n">
+        <v>6.25</v>
+      </c>
     </row>
     <row r="111" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C111" s="14"/>
+      <c r="A111" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B111" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C111" s="14" t="n">
+        <v>42.8125</v>
+      </c>
     </row>
     <row r="112" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C112" s="14"/>
+      <c r="A112" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B112" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C112" s="14" t="n">
+        <v>3.471875</v>
+      </c>
     </row>
     <row r="113" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C113" s="14"/>
+      <c r="A113" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B113" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C113" s="14" t="n">
+        <v>6.25</v>
+      </c>
     </row>
     <row r="114" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C114" s="14"/>
+      <c r="A114" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B114" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C114" s="14" t="n">
+        <v>6.25</v>
+      </c>
     </row>
     <row r="115" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C115" s="14"/>
+      <c r="A115" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B115" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C115" s="14" t="n">
+        <v>6.25</v>
+      </c>
     </row>
     <row r="116" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C116" s="14"/>
+      <c r="A116" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B116" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C116" s="14" t="n">
+        <v>3.125</v>
+      </c>
     </row>
     <row r="117" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C117" s="14"/>
+      <c r="A117" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B117" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C117" s="14" t="n">
+        <v>3.125</v>
+      </c>
     </row>
     <row r="118" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C118" s="14"/>
+      <c r="A118" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B118" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C118" s="14" t="n">
+        <v>3.125</v>
+      </c>
     </row>
     <row r="119" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C119" s="14"/>
+      <c r="A119" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B119" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C119" s="14" t="n">
+        <v>21.40625</v>
+      </c>
     </row>
     <row r="120" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C120" s="14"/>
+      <c r="A120" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B120" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C120" s="14" t="n">
+        <v>1.7359375</v>
+      </c>
     </row>
     <row r="121" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C121" s="14"/>
+      <c r="A121" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B121" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C121" s="14" t="n">
+        <v>3.125</v>
+      </c>
     </row>
     <row r="122" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C122" s="14"/>
+      <c r="A122" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B122" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C122" s="14" t="n">
+        <v>3.125</v>
+      </c>
     </row>
     <row r="123" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C123" s="14"/>
+      <c r="A123" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B123" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C123" s="14" t="n">
+        <v>3.125</v>
+      </c>
     </row>
     <row r="124" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C124" s="14"/>
@@ -4413,22 +4673,13 @@
       <c r="C132" s="14"/>
     </row>
     <row r="133" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A133" s="13"/>
-      <c r="B133" s="13"/>
       <c r="C133" s="14"/>
-      <c r="D133" s="13"/>
     </row>
     <row r="134" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A134" s="13"/>
-      <c r="B134" s="13"/>
       <c r="C134" s="14"/>
-      <c r="D134" s="13"/>
     </row>
     <row r="135" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A135" s="13"/>
-      <c r="B135" s="13"/>
       <c r="C135" s="14"/>
-      <c r="D135" s="13"/>
     </row>
     <row r="136" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C136" s="14"/>
@@ -4437,96 +4688,55 @@
       <c r="C137" s="14"/>
     </row>
     <row r="138" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A138" s="13"/>
-      <c r="B138" s="13"/>
       <c r="C138" s="14"/>
-      <c r="D138" s="13"/>
     </row>
     <row r="139" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A139" s="13"/>
-      <c r="B139" s="13"/>
       <c r="C139" s="14"/>
-      <c r="D139" s="13"/>
     </row>
     <row r="140" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A140" s="13"/>
-      <c r="B140" s="13"/>
       <c r="C140" s="14"/>
-      <c r="D140" s="13"/>
     </row>
     <row r="141" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A141" s="13"/>
-      <c r="B141" s="13"/>
       <c r="C141" s="14"/>
-      <c r="D141" s="13"/>
     </row>
     <row r="142" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A142" s="13"/>
-      <c r="B142" s="13"/>
       <c r="C142" s="14"/>
-      <c r="D142" s="13"/>
     </row>
     <row r="143" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A143" s="13"/>
-      <c r="B143" s="13"/>
       <c r="C143" s="14"/>
-      <c r="D143" s="13"/>
     </row>
     <row r="144" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A144" s="13"/>
-      <c r="B144" s="13"/>
       <c r="C144" s="14"/>
-      <c r="D144" s="13"/>
     </row>
     <row r="145" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A145" s="13"/>
-      <c r="B145" s="13"/>
       <c r="C145" s="14"/>
-      <c r="D145" s="13"/>
     </row>
     <row r="146" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C146" s="14"/>
     </row>
     <row r="147" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A147" s="13"/>
-      <c r="B147" s="13"/>
       <c r="C147" s="14"/>
-      <c r="D147" s="13"/>
     </row>
     <row r="148" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B148" s="13"/>
       <c r="C148" s="14"/>
-      <c r="D148" s="13"/>
     </row>
     <row r="149" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B149" s="13"/>
       <c r="C149" s="14"/>
-      <c r="D149" s="13"/>
     </row>
     <row r="150" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B150" s="13"/>
       <c r="C150" s="14"/>
-      <c r="D150" s="13"/>
     </row>
     <row r="151" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B151" s="13"/>
       <c r="C151" s="14"/>
-      <c r="D151" s="13"/>
     </row>
     <row r="152" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B152" s="13"/>
       <c r="C152" s="14"/>
-      <c r="D152" s="13"/>
     </row>
     <row r="153" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B153" s="13"/>
       <c r="C153" s="14"/>
-      <c r="D153" s="13"/>
     </row>
     <row r="154" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B154" s="13"/>
       <c r="C154" s="14"/>
-      <c r="D154" s="13"/>
     </row>
     <row r="155" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C155" s="14"/>
@@ -7066,7 +7276,16 @@
     <row r="1000" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C1000" s="14"/>
     </row>
+    <row r="1001" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C1001" s="14"/>
+    </row>
+    <row r="1002" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C1002" s="14"/>
+    </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:G1"/>
+  </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -7082,10 +7301,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Q1001"/>
+  <dimension ref="A1:Q1003"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A75" activeCellId="0" sqref="A75"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.4296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -7094,513 +7313,531 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="15" width="10.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="15" width="51.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="4" style="15" width="10.7"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16379" min="18" style="16" width="14.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16380" style="16" width="10.16"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16379" min="18" style="15" width="14.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16380" style="15" width="10.16"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="17" t="s">
-        <v>42</v>
-      </c>
-      <c r="B1" s="18" t="s">
-        <v>68</v>
-      </c>
-      <c r="C1" s="17" t="s">
-        <v>69</v>
-      </c>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
-      <c r="G1" s="17"/>
-      <c r="H1" s="17"/>
-      <c r="I1" s="17"/>
-      <c r="J1" s="17"/>
-      <c r="K1" s="17"/>
-      <c r="L1" s="17"/>
-      <c r="M1" s="17"/>
-      <c r="N1" s="17"/>
-      <c r="O1" s="17"/>
-      <c r="P1" s="17"/>
-      <c r="Q1" s="17"/>
+    <row r="1" customFormat="false" ht="26.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="12"/>
+      <c r="I1" s="12"/>
+      <c r="J1" s="12"/>
+      <c r="K1" s="12"/>
+      <c r="L1" s="12"/>
+      <c r="M1" s="12"/>
+      <c r="N1" s="12"/>
+      <c r="O1" s="12"/>
+      <c r="P1" s="12"/>
+      <c r="Q1" s="12"/>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="15" t="s">
-        <v>70</v>
-      </c>
-      <c r="B2" s="19" t="s">
-        <v>71</v>
-      </c>
-      <c r="C2" s="15" t="s">
-        <v>72</v>
-      </c>
+      <c r="A2" s="12"/>
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="12"/>
+      <c r="H2" s="12"/>
+      <c r="I2" s="12"/>
+      <c r="J2" s="12"/>
+      <c r="K2" s="12"/>
+      <c r="L2" s="12"/>
+      <c r="M2" s="12"/>
+      <c r="N2" s="12"/>
+      <c r="O2" s="12"/>
+      <c r="P2" s="12"/>
+      <c r="Q2" s="12"/>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="15" t="s">
-        <v>45</v>
-      </c>
-      <c r="B3" s="19" t="s">
-        <v>73</v>
-      </c>
-      <c r="C3" s="15" t="s">
-        <v>74</v>
-      </c>
+      <c r="A3" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="D3" s="12"/>
+      <c r="E3" s="12"/>
+      <c r="F3" s="12"/>
+      <c r="G3" s="12"/>
+      <c r="H3" s="12"/>
+      <c r="I3" s="12"/>
+      <c r="J3" s="12"/>
+      <c r="K3" s="12"/>
+      <c r="L3" s="12"/>
+      <c r="M3" s="12"/>
+      <c r="N3" s="12"/>
+      <c r="O3" s="12"/>
+      <c r="P3" s="12"/>
+      <c r="Q3" s="12"/>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="15" t="s">
-        <v>45</v>
-      </c>
-      <c r="B4" s="19" t="s">
-        <v>75</v>
+        <v>77</v>
+      </c>
+      <c r="B4" s="16" t="s">
+        <v>78</v>
       </c>
       <c r="C4" s="15" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="15" t="s">
-        <v>45</v>
-      </c>
-      <c r="B5" s="19" t="s">
-        <v>77</v>
+        <v>46</v>
+      </c>
+      <c r="B5" s="16" t="s">
+        <v>80</v>
       </c>
       <c r="C5" s="15" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="15" t="s">
-        <v>51</v>
-      </c>
-      <c r="B6" s="19" t="s">
-        <v>79</v>
+        <v>46</v>
+      </c>
+      <c r="B6" s="16" t="s">
+        <v>82</v>
       </c>
       <c r="C6" s="15" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="15" t="s">
-        <v>51</v>
-      </c>
-      <c r="B7" s="19" t="s">
-        <v>81</v>
+        <v>46</v>
+      </c>
+      <c r="B7" s="16" t="s">
+        <v>84</v>
       </c>
       <c r="C7" s="15" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="15" t="s">
-        <v>51</v>
-      </c>
-      <c r="B8" s="19" t="s">
-        <v>83</v>
+        <v>52</v>
+      </c>
+      <c r="B8" s="16" t="s">
+        <v>86</v>
       </c>
       <c r="C8" s="15" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="15" t="s">
-        <v>85</v>
-      </c>
-      <c r="B9" s="19" t="s">
-        <v>86</v>
+        <v>52</v>
+      </c>
+      <c r="B9" s="16" t="s">
+        <v>88</v>
       </c>
       <c r="C9" s="15" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="B10" s="19" t="s">
-        <v>88</v>
+      <c r="B10" s="16" t="s">
+        <v>90</v>
       </c>
       <c r="C10" s="15" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="15" t="s">
-        <v>52</v>
-      </c>
-      <c r="B11" s="19" t="s">
-        <v>90</v>
+        <v>92</v>
+      </c>
+      <c r="B11" s="16" t="s">
+        <v>93</v>
       </c>
       <c r="C11" s="15" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="15" t="s">
-        <v>52</v>
-      </c>
-      <c r="B12" s="19" t="s">
-        <v>92</v>
+        <v>53</v>
+      </c>
+      <c r="B12" s="16" t="s">
+        <v>95</v>
       </c>
       <c r="C12" s="15" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="15" t="s">
         <v>53</v>
       </c>
-      <c r="B13" s="19" t="s">
-        <v>94</v>
+      <c r="B13" s="16" t="s">
+        <v>97</v>
       </c>
       <c r="C13" s="15" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="15" t="s">
         <v>53</v>
       </c>
-      <c r="B14" s="19" t="s">
-        <v>96</v>
+      <c r="B14" s="16" t="s">
+        <v>99</v>
       </c>
       <c r="C14" s="15" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="15" t="s">
-        <v>53</v>
-      </c>
-      <c r="B15" s="19" t="s">
-        <v>98</v>
+        <v>54</v>
+      </c>
+      <c r="B15" s="16" t="s">
+        <v>101</v>
       </c>
       <c r="C15" s="15" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="15" t="s">
-        <v>100</v>
-      </c>
-      <c r="B16" s="19" t="s">
-        <v>101</v>
+        <v>54</v>
+      </c>
+      <c r="B16" s="16" t="s">
+        <v>103</v>
       </c>
       <c r="C16" s="15" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="15" t="s">
         <v>54</v>
       </c>
-      <c r="B17" s="19" t="s">
-        <v>103</v>
+      <c r="B17" s="16" t="s">
+        <v>105</v>
       </c>
       <c r="C17" s="15" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="15" t="s">
-        <v>54</v>
-      </c>
-      <c r="B18" s="19" t="s">
-        <v>105</v>
+        <v>107</v>
+      </c>
+      <c r="B18" s="16" t="s">
+        <v>108</v>
       </c>
       <c r="C18" s="15" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="15" t="s">
-        <v>54</v>
-      </c>
-      <c r="B19" s="19" t="s">
-        <v>107</v>
+        <v>55</v>
+      </c>
+      <c r="B19" s="16" t="s">
+        <v>110</v>
       </c>
       <c r="C19" s="15" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="15" t="s">
         <v>55</v>
       </c>
-      <c r="B20" s="19" t="s">
-        <v>109</v>
+      <c r="B20" s="16" t="s">
+        <v>112</v>
       </c>
       <c r="C20" s="15" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="15" t="s">
         <v>55</v>
       </c>
-      <c r="B21" s="19" t="s">
-        <v>111</v>
+      <c r="B21" s="16" t="s">
+        <v>114</v>
       </c>
       <c r="C21" s="15" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="15" t="s">
-        <v>55</v>
-      </c>
-      <c r="B22" s="19" t="s">
-        <v>113</v>
+        <v>56</v>
+      </c>
+      <c r="B22" s="16" t="s">
+        <v>116</v>
       </c>
       <c r="C22" s="15" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="15" t="s">
-        <v>115</v>
-      </c>
-      <c r="B23" s="19" t="s">
-        <v>116</v>
+        <v>56</v>
+      </c>
+      <c r="B23" s="16" t="s">
+        <v>118</v>
       </c>
       <c r="C23" s="15" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="15" t="s">
-        <v>59</v>
-      </c>
-      <c r="B24" s="19" t="s">
-        <v>118</v>
+        <v>56</v>
+      </c>
+      <c r="B24" s="16" t="s">
+        <v>120</v>
       </c>
       <c r="C24" s="15" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="15" t="s">
-        <v>59</v>
-      </c>
-      <c r="B25" s="19" t="s">
-        <v>120</v>
+        <v>122</v>
+      </c>
+      <c r="B25" s="16" t="s">
+        <v>123</v>
       </c>
       <c r="C25" s="15" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="15" t="s">
-        <v>59</v>
-      </c>
-      <c r="B26" s="19" t="s">
-        <v>122</v>
+        <v>60</v>
+      </c>
+      <c r="B26" s="16" t="s">
+        <v>125</v>
       </c>
       <c r="C26" s="15" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="B27" s="19" t="s">
-        <v>124</v>
+      <c r="B27" s="16" t="s">
+        <v>127</v>
       </c>
       <c r="C27" s="15" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="B28" s="19" t="s">
-        <v>126</v>
+      <c r="B28" s="16" t="s">
+        <v>129</v>
       </c>
       <c r="C28" s="15" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="15" t="s">
-        <v>60</v>
-      </c>
-      <c r="B29" s="19" t="s">
-        <v>128</v>
+        <v>61</v>
+      </c>
+      <c r="B29" s="16" t="s">
+        <v>131</v>
       </c>
       <c r="C29" s="15" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="15" t="s">
-        <v>130</v>
-      </c>
-      <c r="B30" s="19" t="s">
-        <v>131</v>
+        <v>61</v>
+      </c>
+      <c r="B30" s="16" t="s">
+        <v>133</v>
       </c>
       <c r="C30" s="15" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="15" t="s">
         <v>61</v>
       </c>
-      <c r="B31" s="19" t="s">
-        <v>133</v>
+      <c r="B31" s="16" t="s">
+        <v>135</v>
       </c>
       <c r="C31" s="15" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="15" t="s">
-        <v>61</v>
-      </c>
-      <c r="B32" s="19" t="s">
-        <v>135</v>
+        <v>137</v>
+      </c>
+      <c r="B32" s="16" t="s">
+        <v>138</v>
       </c>
       <c r="C32" s="15" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="15" t="s">
-        <v>61</v>
-      </c>
-      <c r="B33" s="19" t="s">
-        <v>137</v>
+        <v>62</v>
+      </c>
+      <c r="B33" s="16" t="s">
+        <v>140</v>
       </c>
       <c r="C33" s="15" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="15" t="s">
         <v>62</v>
       </c>
-      <c r="B34" s="19" t="s">
-        <v>139</v>
+      <c r="B34" s="16" t="s">
+        <v>142</v>
       </c>
       <c r="C34" s="15" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="15" t="s">
         <v>62</v>
       </c>
-      <c r="B35" s="19" t="s">
-        <v>141</v>
+      <c r="B35" s="16" t="s">
+        <v>144</v>
       </c>
       <c r="C35" s="15" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="15" t="s">
-        <v>62</v>
-      </c>
-      <c r="B36" s="19" t="s">
-        <v>143</v>
+        <v>63</v>
+      </c>
+      <c r="B36" s="16" t="s">
+        <v>146</v>
       </c>
       <c r="C36" s="15" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="15" t="s">
-        <v>145</v>
-      </c>
-      <c r="B37" s="19" t="s">
-        <v>146</v>
+        <v>63</v>
+      </c>
+      <c r="B37" s="16" t="s">
+        <v>148</v>
       </c>
       <c r="C37" s="15" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="B38" s="19" t="s">
-        <v>148</v>
+        <v>63</v>
+      </c>
+      <c r="B38" s="16" t="s">
+        <v>150</v>
       </c>
       <c r="C38" s="15" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="B39" s="19" t="s">
-        <v>150</v>
+        <v>152</v>
+      </c>
+      <c r="B39" s="16" t="s">
+        <v>153</v>
       </c>
       <c r="C39" s="15" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="15" t="s">
-        <v>31</v>
-      </c>
-      <c r="B40" s="19" t="s">
-        <v>152</v>
+        <v>29</v>
+      </c>
+      <c r="B40" s="16" t="s">
+        <v>155</v>
       </c>
       <c r="C40" s="15" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="15" t="s">
-        <v>154</v>
-      </c>
-      <c r="B41" s="19" t="s">
-        <v>155</v>
+        <v>30</v>
+      </c>
+      <c r="B41" s="16" t="s">
+        <v>157</v>
       </c>
       <c r="C41" s="15" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="15" t="s">
-        <v>154</v>
-      </c>
-      <c r="B42" s="19" t="s">
-        <v>157</v>
+        <v>31</v>
+      </c>
+      <c r="B42" s="16" t="s">
+        <v>159</v>
       </c>
       <c r="C42" s="15" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="15" t="s">
-        <v>154</v>
-      </c>
-      <c r="B43" s="19" t="s">
-        <v>159</v>
+        <v>64</v>
+      </c>
+      <c r="B43" s="16" t="s">
+        <v>161</v>
       </c>
       <c r="C43" s="15" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A44" s="15" t="s">
-        <v>161</v>
-      </c>
-      <c r="B44" s="19" t="s">
-        <v>162</v>
+        <v>64</v>
+      </c>
+      <c r="B44" s="16" t="s">
+        <v>163</v>
       </c>
       <c r="C44" s="15" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A45" s="15" t="s">
-        <v>164</v>
-      </c>
-      <c r="B45" s="19" t="s">
+        <v>64</v>
+      </c>
+      <c r="B45" s="16" t="s">
         <v>165</v>
       </c>
       <c r="C45" s="15" t="s">
@@ -7609,31 +7846,31 @@
     </row>
     <row r="46" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A46" s="15" t="s">
-        <v>164</v>
-      </c>
-      <c r="B46" s="19" t="s">
         <v>167</v>
       </c>
+      <c r="B46" s="16" t="s">
+        <v>168</v>
+      </c>
       <c r="C46" s="15" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A47" s="15" t="s">
-        <v>164</v>
-      </c>
-      <c r="B47" s="19" t="s">
-        <v>169</v>
+        <v>65</v>
+      </c>
+      <c r="B47" s="16" t="s">
+        <v>170</v>
       </c>
       <c r="C47" s="15" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A48" s="15" t="s">
-        <v>171</v>
-      </c>
-      <c r="B48" s="19" t="s">
+        <v>65</v>
+      </c>
+      <c r="B48" s="16" t="s">
         <v>172</v>
       </c>
       <c r="C48" s="15" t="s">
@@ -7642,9 +7879,9 @@
     </row>
     <row r="49" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A49" s="15" t="s">
-        <v>171</v>
-      </c>
-      <c r="B49" s="19" t="s">
+        <v>65</v>
+      </c>
+      <c r="B49" s="16" t="s">
         <v>174</v>
       </c>
       <c r="C49" s="15" t="s">
@@ -7653,9 +7890,9 @@
     </row>
     <row r="50" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A50" s="15" t="s">
-        <v>171</v>
-      </c>
-      <c r="B50" s="19" t="s">
+        <v>66</v>
+      </c>
+      <c r="B50" s="16" t="s">
         <v>176</v>
       </c>
       <c r="C50" s="15" t="s">
@@ -7664,281 +7901,301 @@
     </row>
     <row r="51" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A51" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="B51" s="16" t="s">
         <v>178</v>
       </c>
-      <c r="B51" s="19" t="s">
+      <c r="C51" s="15" t="s">
         <v>179</v>
-      </c>
-      <c r="C51" s="15" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A52" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="B52" s="16" t="s">
+        <v>180</v>
+      </c>
+      <c r="C52" s="15" t="s">
         <v>181</v>
-      </c>
-      <c r="B52" s="19" t="s">
-        <v>182</v>
-      </c>
-      <c r="C52" s="15" t="s">
-        <v>183</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A53" s="15" t="s">
-        <v>181</v>
-      </c>
-      <c r="B53" s="19" t="s">
+        <v>182</v>
+      </c>
+      <c r="B53" s="16" t="s">
+        <v>183</v>
+      </c>
+      <c r="C53" s="15" t="s">
         <v>184</v>
-      </c>
-      <c r="C53" s="15" t="s">
-        <v>185</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A54" s="15" t="s">
-        <v>181</v>
-      </c>
-      <c r="B54" s="19" t="s">
+        <v>67</v>
+      </c>
+      <c r="B54" s="16" t="s">
+        <v>185</v>
+      </c>
+      <c r="C54" s="15" t="s">
         <v>186</v>
-      </c>
-      <c r="C54" s="15" t="s">
-        <v>187</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A55" s="15" t="s">
+        <v>67</v>
+      </c>
+      <c r="B55" s="16" t="s">
+        <v>187</v>
+      </c>
+      <c r="C55" s="15" t="s">
         <v>188</v>
-      </c>
-      <c r="B55" s="19" t="s">
-        <v>189</v>
-      </c>
-      <c r="C55" s="15" t="s">
-        <v>190</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A56" s="15" t="s">
-        <v>188</v>
-      </c>
-      <c r="B56" s="19" t="s">
-        <v>191</v>
+        <v>67</v>
+      </c>
+      <c r="B56" s="16" t="s">
+        <v>189</v>
       </c>
       <c r="C56" s="15" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A57" s="15" t="s">
-        <v>188</v>
-      </c>
-      <c r="B57" s="19" t="s">
-        <v>193</v>
+        <v>68</v>
+      </c>
+      <c r="B57" s="16" t="s">
+        <v>191</v>
       </c>
       <c r="C57" s="15" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A58" s="15" t="s">
-        <v>195</v>
-      </c>
-      <c r="B58" s="19" t="s">
-        <v>196</v>
+        <v>68</v>
+      </c>
+      <c r="B58" s="16" t="s">
+        <v>193</v>
       </c>
       <c r="C58" s="15" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A59" s="15" t="s">
-        <v>198</v>
-      </c>
-      <c r="B59" s="19" t="s">
-        <v>199</v>
+        <v>68</v>
+      </c>
+      <c r="B59" s="16" t="s">
+        <v>195</v>
       </c>
       <c r="C59" s="15" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A60" s="15" t="s">
+        <v>197</v>
+      </c>
+      <c r="B60" s="16" t="s">
         <v>198</v>
       </c>
-      <c r="B60" s="19" t="s">
-        <v>201</v>
-      </c>
       <c r="C60" s="15" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A61" s="15" t="s">
-        <v>198</v>
-      </c>
-      <c r="B61" s="19" t="s">
-        <v>203</v>
+        <v>69</v>
+      </c>
+      <c r="B61" s="16" t="s">
+        <v>200</v>
       </c>
       <c r="C61" s="15" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A62" s="15" t="s">
-        <v>205</v>
-      </c>
-      <c r="B62" s="19" t="s">
-        <v>206</v>
+        <v>69</v>
+      </c>
+      <c r="B62" s="16" t="s">
+        <v>202</v>
       </c>
       <c r="C62" s="15" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A63" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="B63" s="16" t="s">
+        <v>204</v>
+      </c>
+      <c r="C63" s="15" t="s">
         <v>205</v>
-      </c>
-      <c r="B63" s="19" t="s">
-        <v>208</v>
-      </c>
-      <c r="C63" s="15" t="s">
-        <v>209</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A64" s="15" t="s">
-        <v>205</v>
-      </c>
-      <c r="B64" s="19" t="s">
-        <v>210</v>
+        <v>70</v>
+      </c>
+      <c r="B64" s="16" t="s">
+        <v>206</v>
       </c>
       <c r="C64" s="15" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A65" s="15" t="s">
-        <v>212</v>
-      </c>
-      <c r="B65" s="19" t="s">
-        <v>213</v>
+        <v>70</v>
+      </c>
+      <c r="B65" s="16" t="s">
+        <v>208</v>
       </c>
       <c r="C65" s="15" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A66" s="15" t="s">
-        <v>215</v>
-      </c>
-      <c r="B66" s="19" t="s">
-        <v>216</v>
+        <v>70</v>
+      </c>
+      <c r="B66" s="16" t="s">
+        <v>210</v>
       </c>
       <c r="C66" s="15" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A67" s="15" t="s">
-        <v>215</v>
-      </c>
-      <c r="B67" s="19" t="s">
-        <v>218</v>
+        <v>212</v>
+      </c>
+      <c r="B67" s="16" t="s">
+        <v>213</v>
       </c>
       <c r="C67" s="15" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A68" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="B68" s="16" t="s">
         <v>215</v>
       </c>
-      <c r="B68" s="19" t="s">
-        <v>220</v>
-      </c>
       <c r="C68" s="15" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A69" s="15" t="s">
-        <v>222</v>
-      </c>
-      <c r="B69" s="19" t="s">
-        <v>223</v>
+        <v>71</v>
+      </c>
+      <c r="B69" s="16" t="s">
+        <v>217</v>
       </c>
       <c r="C69" s="15" t="s">
-        <v>224</v>
+        <v>218</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A70" s="15" t="s">
-        <v>222</v>
-      </c>
-      <c r="B70" s="19" t="s">
-        <v>225</v>
+        <v>71</v>
+      </c>
+      <c r="B70" s="16" t="s">
+        <v>219</v>
       </c>
       <c r="C70" s="15" t="s">
-        <v>226</v>
+        <v>220</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A71" s="15" t="s">
+        <v>72</v>
+      </c>
+      <c r="B71" s="16" t="s">
+        <v>221</v>
+      </c>
+      <c r="C71" s="15" t="s">
         <v>222</v>
-      </c>
-      <c r="B71" s="19" t="s">
-        <v>227</v>
-      </c>
-      <c r="C71" s="15" t="s">
-        <v>228</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A72" s="15" t="s">
-        <v>229</v>
-      </c>
-      <c r="B72" s="19" t="s">
-        <v>230</v>
+        <v>72</v>
+      </c>
+      <c r="B72" s="16" t="s">
+        <v>223</v>
       </c>
       <c r="C72" s="15" t="s">
-        <v>231</v>
+        <v>224</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A73" s="15" t="s">
-        <v>232</v>
-      </c>
-      <c r="B73" s="19" t="s">
-        <v>233</v>
+        <v>72</v>
+      </c>
+      <c r="B73" s="16" t="s">
+        <v>225</v>
       </c>
       <c r="C73" s="15" t="s">
-        <v>234</v>
+        <v>226</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A74" s="15" t="s">
-        <v>232</v>
-      </c>
-      <c r="B74" s="19" t="s">
-        <v>235</v>
+        <v>227</v>
+      </c>
+      <c r="B74" s="16" t="s">
+        <v>228</v>
       </c>
       <c r="C74" s="15" t="s">
-        <v>236</v>
+        <v>229</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A75" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="B75" s="16" t="s">
+        <v>230</v>
+      </c>
+      <c r="C75" s="15" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="76" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A76" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="B76" s="16" t="s">
         <v>232</v>
       </c>
-      <c r="B75" s="19" t="s">
-        <v>237</v>
-      </c>
-      <c r="C75" s="15" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="76" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="77" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+      <c r="C76" s="15" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="77" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A77" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="B77" s="16" t="s">
+        <v>234</v>
+      </c>
+      <c r="C77" s="15" t="s">
+        <v>235</v>
+      </c>
+    </row>
     <row r="78" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="79" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="80" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -8863,7 +9120,12 @@
     <row r="999" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1000" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1001" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1002" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1003" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:G1"/>
+  </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>